<commit_message>
excel data driven test modified
</commit_message>
<xml_diff>
--- a/excel-test-data/test-data.xlsx
+++ b/excel-test-data/test-data.xlsx
@@ -11,30 +11,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Username</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>MobileNo</t>
-  </si>
-  <si>
-    <t>Michael Jordan</t>
-  </si>
-  <si>
-    <t>Mjordan</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Bulls Blvd</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>United States of America (the)</t>
   </si>
   <si>
     <r>
@@ -44,28 +71,20 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>jordan@test.com</t>
+      <t>mjordan@test.com</t>
     </r>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Kobe Bryant</t>
-  </si>
-  <si>
-    <t>Kbryant</t>
-  </si>
-  <si>
-    <t>kobe@test.com</t>
+    <t>Mj1093nciqo!@s9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="yyyy-m-d"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -122,7 +141,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -130,6 +149,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1184,14 +1206,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="11" width="16.3516" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.05" customHeight="1">
@@ -1213,194 +1235,294 @@
       <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" s="3">
-        <v>1</v>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" ht="32.05" customHeight="1">
+      <c r="A2" t="s" s="2">
+        <v>11</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30314</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3">
-        <v>4071234567</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="4">
+        <v>21998</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4">
+        <v>4079998877</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3">
-        <v>4079998877</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="" tooltip="" display="jordan@test.com"/>
+    <hyperlink ref="J2" r:id="rId1" location="" tooltip="" display="mjordan@test.com"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>